<commit_message>
Updated with Mark Steffensen's changes to support 2023.4
</commit_message>
<xml_diff>
--- a/05_ObjectRepository/Default.xlsx
+++ b/05_ObjectRepository/Default.xlsx
@@ -469,14 +469,11 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16383" width="8.8984375" style="1" customWidth="1"/>
-    <col min="16384" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>